<commit_message>
colorful area difference in excel
</commit_message>
<xml_diff>
--- a/Planbeispiele_mit_Flaechen/P19101721004/Flächen vergleich.xlsx
+++ b/Planbeispiele_mit_Flaechen/P19101721004/Flächen vergleich.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FHNW\semester_7\3_IP6\IP6_ModellingBuildingEnvelopes\Planbeispiele_mit_Flaechen\P19101721004\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BA25F8-6C9E-4104-8502-9BA7AAB866EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B9FCED-10B8-4151-B4EE-5780022C1E86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="54">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>Sketchup</t>
+  </si>
+  <si>
+    <t>Differenz</t>
+  </si>
+  <si>
+    <t>BO1/BO2/BO3</t>
   </si>
 </sst>
 </file>
@@ -515,7 +521,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -734,6 +740,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -779,7 +798,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -805,6 +824,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1160,10 +1180,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:S54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F21" workbookViewId="0">
-      <selection activeCell="U37" sqref="U37"/>
+    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U50" sqref="U50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2053,7 +2073,18 @@
       </c>
       <c r="S32" s="14"/>
     </row>
-    <row r="34" spans="11:18" x14ac:dyDescent="0.45">
+    <row r="33" spans="11:19" x14ac:dyDescent="0.45">
+      <c r="K33" s="9"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="9"/>
+      <c r="S33" s="9"/>
+    </row>
+    <row r="34" spans="11:19" x14ac:dyDescent="0.45">
       <c r="K34" s="15"/>
       <c r="L34" s="3"/>
       <c r="M34" s="2" t="s">
@@ -2071,7 +2102,7 @@
       <c r="Q34" s="3"/>
       <c r="R34" s="16"/>
     </row>
-    <row r="35" spans="11:18" x14ac:dyDescent="0.45">
+    <row r="35" spans="11:19" x14ac:dyDescent="0.45">
       <c r="K35" s="17" t="s">
         <v>51</v>
       </c>
@@ -2095,101 +2126,95 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="11:18" x14ac:dyDescent="0.45">
+    <row r="36" spans="11:19" x14ac:dyDescent="0.45">
       <c r="K36" s="19"/>
       <c r="L36" s="8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="M36" s="9">
-        <v>107.31</v>
+        <v>12.46</v>
       </c>
       <c r="N36" s="9">
-        <v>40.630000000000003</v>
+        <v>1.66</v>
       </c>
       <c r="O36" s="9">
-        <v>40.03</v>
+        <v>1.55</v>
       </c>
       <c r="P36" s="9">
-        <v>96.63</v>
-      </c>
-      <c r="Q36" s="9"/>
+        <v>29.75</v>
+      </c>
+      <c r="Q36" s="9">
+        <v>5.32</v>
+      </c>
       <c r="R36" s="10">
-        <v>284.60000000000002</v>
-      </c>
-    </row>
-    <row r="37" spans="11:18" x14ac:dyDescent="0.45">
+        <v>50.74</v>
+      </c>
+    </row>
+    <row r="37" spans="11:19" x14ac:dyDescent="0.45">
       <c r="K37" s="19"/>
       <c r="L37" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="M37" s="9"/>
+        <v>48</v>
+      </c>
+      <c r="M37" s="9">
+        <v>5.39</v>
+      </c>
       <c r="N37" s="9"/>
-      <c r="O37" s="9">
-        <v>7.13</v>
-      </c>
+      <c r="O37" s="9"/>
       <c r="P37" s="9"/>
       <c r="Q37" s="9"/>
       <c r="R37" s="10">
-        <v>7.13</v>
-      </c>
-    </row>
-    <row r="38" spans="11:18" x14ac:dyDescent="0.45">
+        <v>5.39</v>
+      </c>
+    </row>
+    <row r="38" spans="11:19" x14ac:dyDescent="0.45">
       <c r="K38" s="19"/>
-      <c r="L38" s="8" t="s">
-        <v>46</v>
-      </c>
+      <c r="L38" s="8"/>
       <c r="M38" s="9"/>
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
       <c r="P38" s="9"/>
-      <c r="Q38" s="9">
-        <v>115.52</v>
-      </c>
-      <c r="R38" s="10">
-        <v>115.52</v>
-      </c>
-    </row>
-    <row r="39" spans="11:18" x14ac:dyDescent="0.45">
+      <c r="Q38" s="9"/>
+      <c r="R38" s="10"/>
+    </row>
+    <row r="39" spans="11:19" x14ac:dyDescent="0.45">
       <c r="K39" s="19"/>
       <c r="L39" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M39" s="9">
-        <v>12.46</v>
+        <v>107.31</v>
       </c>
       <c r="N39" s="9">
-        <v>1.66</v>
+        <v>40.630000000000003</v>
       </c>
       <c r="O39" s="9">
-        <v>1.55</v>
+        <v>40.03</v>
       </c>
       <c r="P39" s="9">
-        <v>29.75</v>
-      </c>
-      <c r="Q39" s="9">
-        <v>5.32</v>
-      </c>
+        <v>96.63</v>
+      </c>
+      <c r="Q39" s="9"/>
       <c r="R39" s="10">
-        <v>50.74</v>
-      </c>
-    </row>
-    <row r="40" spans="11:18" x14ac:dyDescent="0.45">
+        <v>284.60000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="11:19" x14ac:dyDescent="0.45">
       <c r="K40" s="19"/>
       <c r="L40" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M40" s="9">
-        <v>5.39</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="M40" s="9"/>
       <c r="N40" s="9"/>
-      <c r="O40" s="9"/>
+      <c r="O40" s="9">
+        <v>7.13</v>
+      </c>
       <c r="P40" s="9"/>
       <c r="Q40" s="9"/>
       <c r="R40" s="10">
-        <v>5.39</v>
-      </c>
-    </row>
-    <row r="41" spans="11:18" x14ac:dyDescent="0.45">
+        <v>7.13</v>
+      </c>
+    </row>
+    <row r="41" spans="11:19" x14ac:dyDescent="0.45">
       <c r="K41" s="19"/>
       <c r="L41" s="8" t="s">
         <v>49</v>
@@ -2207,34 +2232,333 @@
         <v>136.53</v>
       </c>
     </row>
-    <row r="42" spans="11:18" x14ac:dyDescent="0.45">
-      <c r="K42" s="11"/>
-      <c r="L42" s="20" t="s">
+    <row r="42" spans="11:19" x14ac:dyDescent="0.45">
+      <c r="K42" s="19"/>
+      <c r="L42" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="9"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="9">
+        <v>115.52</v>
+      </c>
+      <c r="R42" s="10">
+        <v>115.52</v>
+      </c>
+    </row>
+    <row r="43" spans="11:19" x14ac:dyDescent="0.45">
+      <c r="K43" s="23"/>
+      <c r="L43" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="M42" s="21">
+      <c r="M43" s="21">
         <v>125.16</v>
       </c>
-      <c r="N42" s="21">
+      <c r="N43" s="21">
         <v>42.29</v>
       </c>
-      <c r="O42" s="21">
+      <c r="O43" s="21">
         <v>48.71</v>
       </c>
-      <c r="P42" s="21">
+      <c r="P43" s="21">
         <v>126.52</v>
       </c>
-      <c r="Q42" s="21">
+      <c r="Q43" s="21">
         <v>257.24</v>
       </c>
-      <c r="R42" s="22">
+      <c r="R43" s="22">
         <v>599.91</v>
       </c>
     </row>
-    <row r="43" spans="11:18" x14ac:dyDescent="0.45">
-      <c r="L43" s="1"/>
+    <row r="44" spans="11:19" x14ac:dyDescent="0.45">
+      <c r="L44" s="1"/>
+    </row>
+    <row r="45" spans="11:19" x14ac:dyDescent="0.45">
+      <c r="K45" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="16"/>
+    </row>
+    <row r="46" spans="11:19" x14ac:dyDescent="0.45">
+      <c r="K46" s="19"/>
+      <c r="L46" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M46" s="9">
+        <f>IF(M36-M23=0,"",M36-M23)</f>
+        <v>-6.07</v>
+      </c>
+      <c r="N46" s="9">
+        <f t="shared" ref="N46:R46" si="1">IF(N36-N23=0,"",N36-N23)</f>
+        <v>-3.84</v>
+      </c>
+      <c r="O46" s="9">
+        <f t="shared" si="1"/>
+        <v>-6.05</v>
+      </c>
+      <c r="P46" s="9">
+        <f t="shared" si="1"/>
+        <v>-1.1499999999999986</v>
+      </c>
+      <c r="Q46" s="9">
+        <f t="shared" si="1"/>
+        <v>5.32</v>
+      </c>
+      <c r="R46" s="10">
+        <f t="shared" si="1"/>
+        <v>-11.79</v>
+      </c>
+    </row>
+    <row r="47" spans="11:19" x14ac:dyDescent="0.45">
+      <c r="K47" s="19"/>
+      <c r="L47" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="M47" s="9">
+        <f t="shared" ref="M47:R47" si="2">IF(M37-M24=0,"",M37-M24)</f>
+        <v>-0.28000000000000025</v>
+      </c>
+      <c r="N47" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O47" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P47" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="Q47" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="R47" s="10">
+        <f t="shared" si="2"/>
+        <v>-0.28000000000000025</v>
+      </c>
+    </row>
+    <row r="48" spans="11:19" x14ac:dyDescent="0.45">
+      <c r="K48" s="19"/>
+      <c r="L48" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="M48" s="9">
+        <f t="shared" ref="M48:R48" si="3">IF(M38-M25=0,"",M38-M25)</f>
+        <v>-2</v>
+      </c>
+      <c r="N48" s="9">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="O48" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="P48" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="Q48" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="R48" s="10">
+        <f t="shared" si="3"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="49" spans="11:18" x14ac:dyDescent="0.45">
+      <c r="K49" s="19"/>
+      <c r="L49" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M49" s="9">
+        <f t="shared" ref="M49:R49" si="4">IF(M39-M26=0,"",M39-M26)</f>
+        <v>8.8100000000000023</v>
+      </c>
+      <c r="N49" s="9">
+        <f t="shared" si="4"/>
+        <v>3.0000000000001137E-2</v>
+      </c>
+      <c r="O49" s="9">
+        <f t="shared" si="4"/>
+        <v>1.4299999999999997</v>
+      </c>
+      <c r="P49" s="9">
+        <f t="shared" si="4"/>
+        <v>4.9299999999999926</v>
+      </c>
+      <c r="Q49" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R49" s="10">
+        <f t="shared" si="4"/>
+        <v>15.200000000000045</v>
+      </c>
+    </row>
+    <row r="50" spans="11:18" x14ac:dyDescent="0.45">
+      <c r="K50" s="19"/>
+      <c r="L50" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M50" s="9">
+        <f t="shared" ref="M50:R50" si="5">IF(M40-M27=0,"",M40-M27)</f>
+        <v>-13.5</v>
+      </c>
+      <c r="N50" s="9">
+        <f t="shared" si="5"/>
+        <v>-4</v>
+      </c>
+      <c r="O50" s="9">
+        <f t="shared" si="5"/>
+        <v>3.23</v>
+      </c>
+      <c r="P50" s="9">
+        <f t="shared" si="5"/>
+        <v>-13.5</v>
+      </c>
+      <c r="Q50" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="R50" s="10">
+        <f t="shared" si="5"/>
+        <v>-27.77</v>
+      </c>
+    </row>
+    <row r="51" spans="11:18" x14ac:dyDescent="0.45">
+      <c r="K51" s="19"/>
+      <c r="L51" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="M51" s="9">
+        <f t="shared" ref="M51:R52" si="6">IF(M41-M28=0,"",M41-M28)</f>
+        <v>-66.3</v>
+      </c>
+      <c r="N51" s="9">
+        <f t="shared" si="6"/>
+        <v>-65.8</v>
+      </c>
+      <c r="O51" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="P51" s="9">
+        <f t="shared" si="6"/>
+        <v>0.13</v>
+      </c>
+      <c r="Q51" s="9">
+        <f t="shared" si="6"/>
+        <v>136.4</v>
+      </c>
+      <c r="R51" s="10">
+        <f t="shared" si="6"/>
+        <v>4.4300000000000068</v>
+      </c>
+    </row>
+    <row r="52" spans="11:18" x14ac:dyDescent="0.45">
+      <c r="K52" s="19"/>
+      <c r="L52" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="M52" s="9" t="str">
+        <f>IF(M42-SUM(M29:M31)=0,"",M42-SUM(M29:M31))</f>
+        <v/>
+      </c>
+      <c r="N52" s="9" t="str">
+        <f t="shared" ref="N52:R52" si="7">IF(N42-SUM(N29:N31)=0,"",N42-SUM(N29:N31))</f>
+        <v/>
+      </c>
+      <c r="O52" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="P52" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="Q52" s="9">
+        <f t="shared" si="7"/>
+        <v>-1.8800000000000097</v>
+      </c>
+      <c r="R52" s="10">
+        <f t="shared" si="7"/>
+        <v>-1.8800000000000097</v>
+      </c>
+    </row>
+    <row r="53" spans="11:18" x14ac:dyDescent="0.45">
+      <c r="K53" s="23"/>
+      <c r="L53" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="M53" s="21">
+        <f>IF(M43-M32=0,"",M43-M32)</f>
+        <v>-79.34</v>
+      </c>
+      <c r="N53" s="21">
+        <f t="shared" ref="N53:R53" si="8">IF(N43-N32=0,"",N43-N32)</f>
+        <v>-75.610000000000014</v>
+      </c>
+      <c r="O53" s="21">
+        <f t="shared" si="8"/>
+        <v>-1.3900000000000006</v>
+      </c>
+      <c r="P53" s="21">
+        <f t="shared" si="8"/>
+        <v>-9.5799999999999983</v>
+      </c>
+      <c r="Q53" s="21">
+        <f t="shared" si="8"/>
+        <v>139.84</v>
+      </c>
+      <c r="R53" s="22">
+        <f t="shared" si="8"/>
+        <v>-26.089999999999918</v>
+      </c>
+    </row>
+    <row r="54" spans="11:18" x14ac:dyDescent="0.45">
+      <c r="L54" s="8"/>
+      <c r="M54" t="str">
+        <f t="shared" ref="M54:R54" si="9">IF(M44-M31=0,"",M44-M31)</f>
+        <v/>
+      </c>
+      <c r="N54" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O54" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="P54" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="M46:R53">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>

</xml_diff>